<commit_message>
New template and fix of soil_depth options
</commit_message>
<xml_diff>
--- a/static/xls/template_with_dropdowns_for_one_drive_and_excel.xlsx
+++ b/static/xls/template_with_dropdowns_for_one_drive_and_excel.xlsx
@@ -445,57 +445,57 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>Elevation</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Vegetation</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Land_use</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Agricultural_land</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Ecosystem</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Grid_Size</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Soil_depth</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Transport_refrigeration</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>Drying</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>Date_collected</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>DNA_concentration_ng_ul</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Elevation</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
@@ -616,26 +616,26 @@
     <row r="101"/>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation sqref="F2 F3 F4 F5 F6 F7 F8 F9 F10 F11 F12 F13 F14 F15 F16 F17 F18 F19 F20 F21 F22 F23 F24 F25 F26 F27 F28 F29 F30 F31 F32 F33 F34 F35 F36 F37 F38 F39 F40 F41 F42 F43 F44 F45 F46 F47 F48 F49 F50 F51 F52 F53 F54 F55 F56 F57 F58 F59 F60 F61 F62 F63 F64 F65 F66 F67 F68 F69 F70 F71 F72 F73 F74 F75 F76 F77 F78 F79 F80 F81 F82 F83 F84 F85 F86 F87 F88 F89 F90 F91 F92 F93 F94 F95 F96 F97 F98 F99 F100 F101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Options!$F$1:$F$11</formula1>
-    </dataValidation>
     <dataValidation sqref="G2 G3 G4 G5 G6 G7 G8 G9 G10 G11 G12 G13 G14 G15 G16 G17 G18 G19 G20 G21 G22 G23 G24 G25 G26 G27 G28 G29 G30 G31 G32 G33 G34 G35 G36 G37 G38 G39 G40 G41 G42 G43 G44 G45 G46 G47 G48 G49 G50 G51 G52 G53 G54 G55 G56 G57 G58 G59 G60 G61 G62 G63 G64 G65 G66 G67 G68 G69 G70 G71 G72 G73 G74 G75 G76 G77 G78 G79 G80 G81 G82 G83 G84 G85 G86 G87 G88 G89 G90 G91 G92 G93 G94 G95 G96 G97 G98 G99 G100 G101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Options!$G$1:$G$2</formula1>
+      <formula1>=Options!$G$1:$G$11</formula1>
     </dataValidation>
     <dataValidation sqref="H2 H3 H4 H5 H6 H7 H8 H9 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21 H22 H23 H24 H25 H26 H27 H28 H29 H30 H31 H32 H33 H34 H35 H36 H37 H38 H39 H40 H41 H42 H43 H44 H45 H46 H47 H48 H49 H50 H51 H52 H53 H54 H55 H56 H57 H58 H59 H60 H61 H62 H63 H64 H65 H66 H67 H68 H69 H70 H71 H72 H73 H74 H75 H76 H77 H78 H79 H80 H81 H82 H83 H84 H85 H86 H87 H88 H89 H90 H91 H92 H93 H94 H95 H96 H97 H98 H99 H100 H101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Options!$H$1:$H$14</formula1>
+      <formula1>=Options!$H$1:$H$2</formula1>
     </dataValidation>
     <dataValidation sqref="I2 I3 I4 I5 I6 I7 I8 I9 I10 I11 I12 I13 I14 I15 I16 I17 I18 I19 I20 I21 I22 I23 I24 I25 I26 I27 I28 I29 I30 I31 I32 I33 I34 I35 I36 I37 I38 I39 I40 I41 I42 I43 I44 I45 I46 I47 I48 I49 I50 I51 I52 I53 I54 I55 I56 I57 I58 I59 I60 I61 I62 I63 I64 I65 I66 I67 I68 I69 I70 I71 I72 I73 I74 I75 I76 I77 I78 I79 I80 I81 I82 I83 I84 I85 I86 I87 I88 I89 I90 I91 I92 I93 I94 I95 I96 I97 I98 I99 I100 I101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Options!$I$1:$I$4</formula1>
+      <formula1>=Options!$I$1:$I$14</formula1>
     </dataValidation>
     <dataValidation sqref="J2 J3 J4 J5 J6 J7 J8 J9 J10 J11 J12 J13 J14 J15 J16 J17 J18 J19 J20 J21 J22 J23 J24 J25 J26 J27 J28 J29 J30 J31 J32 J33 J34 J35 J36 J37 J38 J39 J40 J41 J42 J43 J44 J45 J46 J47 J48 J49 J50 J51 J52 J53 J54 J55 J56 J57 J58 J59 J60 J61 J62 J63 J64 J65 J66 J67 J68 J69 J70 J71 J72 J73 J74 J75 J76 J77 J78 J79 J80 J81 J82 J83 J84 J85 J86 J87 J88 J89 J90 J91 J92 J93 J94 J95 J96 J97 J98 J99 J100 J101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Options!$J$1:$J$5</formula1>
+      <formula1>=Options!$J$1:$J$4</formula1>
     </dataValidation>
     <dataValidation sqref="K2 K3 K4 K5 K6 K7 K8 K9 K10 K11 K12 K13 K14 K15 K16 K17 K18 K19 K20 K21 K22 K23 K24 K25 K26 K27 K28 K29 K30 K31 K32 K33 K34 K35 K36 K37 K38 K39 K40 K41 K42 K43 K44 K45 K46 K47 K48 K49 K50 K51 K52 K53 K54 K55 K56 K57 K58 K59 K60 K61 K62 K63 K64 K65 K66 K67 K68 K69 K70 K71 K72 K73 K74 K75 K76 K77 K78 K79 K80 K81 K82 K83 K84 K85 K86 K87 K88 K89 K90 K91 K92 K93 K94 K95 K96 K97 K98 K99 K100 K101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Options!$K$1:$K$3</formula1>
+      <formula1>=Options!$K$1:$K$5</formula1>
     </dataValidation>
     <dataValidation sqref="L2 L3 L4 L5 L6 L7 L8 L9 L10 L11 L12 L13 L14 L15 L16 L17 L18 L19 L20 L21 L22 L23 L24 L25 L26 L27 L28 L29 L30 L31 L32 L33 L34 L35 L36 L37 L38 L39 L40 L41 L42 L43 L44 L45 L46 L47 L48 L49 L50 L51 L52 L53 L54 L55 L56 L57 L58 L59 L60 L61 L62 L63 L64 L65 L66 L67 L68 L69 L70 L71 L72 L73 L74 L75 L76 L77 L78 L79 L80 L81 L82 L83 L84 L85 L86 L87 L88 L89 L90 L91 L92 L93 L94 L95 L96 L97 L98 L99 L100 L101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Options!$L$1:$L$4</formula1>
+      <formula1>=Options!$L$1:$L$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2 M3 M4 M5 M6 M7 M8 M9 M10 M11 M12 M13 M14 M15 M16 M17 M18 M19 M20 M21 M22 M23 M24 M25 M26 M27 M28 M29 M30 M31 M32 M33 M34 M35 M36 M37 M38 M39 M40 M41 M42 M43 M44 M45 M46 M47 M48 M49 M50 M51 M52 M53 M54 M55 M56 M57 M58 M59 M60 M61 M62 M63 M64 M65 M66 M67 M68 M69 M70 M71 M72 M73 M74 M75 M76 M77 M78 M79 M80 M81 M82 M83 M84 M85 M86 M87 M88 M89 M90 M91 M92 M93 M94 M95 M96 M97 M98 M99 M100 M101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=Options!$M$1:$M$4</formula1>
     </dataValidation>
     <dataValidation sqref="P2 P3 P4 P5 P6 P7 P8 P9 P10 P11 P12 P13 P14 P15 P16 P17 P18 P19 P20 P21 P22 P23 P24 P25 P26 P27 P28 P29 P30 P31 P32 P33 P34 P35 P36 P37 P38 P39 P40 P41 P42 P43 P44 P45 P46 P47 P48 P49 P50 P51 P52 P53 P54 P55 P56 P57 P58 P59 P60 P61 P62 P63 P64 P65 P66 P67 P68 P69 P70 P71 P72 P73 P74 P75 P76 P77 P78 P79 P80 P81 P82 P83 P84 P85 P86 P87 P88 P89 P90 P91 P92 P93 P94 P95 P96 P97 P98 P99 P100 P101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>=Options!$P$1:$P$2</formula1>
@@ -651,7 +651,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="F1:P14"/>
+  <dimension ref="G1:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -660,37 +660,37 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>trees</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Boreal Forests/Taiga</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>10m</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>5-10cm</t>
-        </is>
-      </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>0-10cm</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>Airdrying up to 24h</t>
         </is>
@@ -702,37 +702,37 @@
       </c>
     </row>
     <row r="2">
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>shrubs</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Deserts &amp; Xeric Shrublands</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>20m</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>10-15cm</t>
-        </is>
-      </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>10-20cm</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
           <t>No</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>Airdrying 24h-48h</t>
         </is>
@@ -744,169 +744,169 @@
       </c>
     </row>
     <row r="3">
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>grassland</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Flooded Grasslands &amp; Savannas</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>30m</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>15cm-30cm</t>
-        </is>
-      </c>
       <c r="K3" t="inlineStr">
         <is>
+          <t>20cm-30cm</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
           <t>Yes, refrigeration up to 24h after collection</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>Airdrying 48h+</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>cropland</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Mangroves</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>Other (specify in notes)</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>30cm-1m</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>built up</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Mediterranean Forests, Woodlands &amp; Scrub</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>1m+</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>bare/spare vegetation</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Montane Grasslands &amp; Shrublands</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>snow/ice</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Temperate Broadleaf &amp; Mixed Forests</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>water body</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>Temperate Conifer Forests</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>herbaceous wetland</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>Temperate Grasslands, Savannas &amp; Shrublands</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>mangrove</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>Tropical &amp; Subtropical Coniferous Forests</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>moss/lichen</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Tropical &amp; Subtropical Dry Broadleaf Forests</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>Tropical &amp; Subtropical Grasslands, Savannas &amp; Shrublands</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>Tropical &amp; Subtropical Moist Broadleaf Forests</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>Tundra</t>
         </is>

</xml_diff>

<commit_message>
Add field for sample_type
</commit_message>
<xml_diff>
--- a/static/xls/template_with_dropdowns_for_one_drive_and_excel.xlsx
+++ b/static/xls/template_with_dropdowns_for_one_drive_and_excel.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R101"/>
+  <dimension ref="A1:S101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,15 +500,20 @@
       </c>
       <c r="P1" t="inlineStr">
         <is>
+          <t>Sample_type</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
           <t>Sample_or_Control</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>SequencingRun</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
@@ -615,15 +620,15 @@
     <row r="100"/>
     <row r="101"/>
   </sheetData>
-  <dataValidations count="8">
+  <dataValidations count="9">
     <dataValidation sqref="G2 G3 G4 G5 G6 G7 G8 G9 G10 G11 G12 G13 G14 G15 G16 G17 G18 G19 G20 G21 G22 G23 G24 G25 G26 G27 G28 G29 G30 G31 G32 G33 G34 G35 G36 G37 G38 G39 G40 G41 G42 G43 G44 G45 G46 G47 G48 G49 G50 G51 G52 G53 G54 G55 G56 G57 G58 G59 G60 G61 G62 G63 G64 G65 G66 G67 G68 G69 G70 G71 G72 G73 G74 G75 G76 G77 G78 G79 G80 G81 G82 G83 G84 G85 G86 G87 G88 G89 G90 G91 G92 G93 G94 G95 G96 G97 G98 G99 G100 G101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Options!$G$1:$G$11</formula1>
+      <formula1>=Options!$G$1:$G$12</formula1>
     </dataValidation>
     <dataValidation sqref="H2 H3 H4 H5 H6 H7 H8 H9 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21 H22 H23 H24 H25 H26 H27 H28 H29 H30 H31 H32 H33 H34 H35 H36 H37 H38 H39 H40 H41 H42 H43 H44 H45 H46 H47 H48 H49 H50 H51 H52 H53 H54 H55 H56 H57 H58 H59 H60 H61 H62 H63 H64 H65 H66 H67 H68 H69 H70 H71 H72 H73 H74 H75 H76 H77 H78 H79 H80 H81 H82 H83 H84 H85 H86 H87 H88 H89 H90 H91 H92 H93 H94 H95 H96 H97 H98 H99 H100 H101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Options!$H$1:$H$2</formula1>
+      <formula1>=Options!$H$1:$H$3</formula1>
     </dataValidation>
     <dataValidation sqref="I2 I3 I4 I5 I6 I7 I8 I9 I10 I11 I12 I13 I14 I15 I16 I17 I18 I19 I20 I21 I22 I23 I24 I25 I26 I27 I28 I29 I30 I31 I32 I33 I34 I35 I36 I37 I38 I39 I40 I41 I42 I43 I44 I45 I46 I47 I48 I49 I50 I51 I52 I53 I54 I55 I56 I57 I58 I59 I60 I61 I62 I63 I64 I65 I66 I67 I68 I69 I70 I71 I72 I73 I74 I75 I76 I77 I78 I79 I80 I81 I82 I83 I84 I85 I86 I87 I88 I89 I90 I91 I92 I93 I94 I95 I96 I97 I98 I99 I100 I101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Options!$I$1:$I$14</formula1>
+      <formula1>=Options!$I$1:$I$15</formula1>
     </dataValidation>
     <dataValidation sqref="J2 J3 J4 J5 J6 J7 J8 J9 J10 J11 J12 J13 J14 J15 J16 J17 J18 J19 J20 J21 J22 J23 J24 J25 J26 J27 J28 J29 J30 J31 J32 J33 J34 J35 J36 J37 J38 J39 J40 J41 J42 J43 J44 J45 J46 J47 J48 J49 J50 J51 J52 J53 J54 J55 J56 J57 J58 J59 J60 J61 J62 J63 J64 J65 J66 J67 J68 J69 J70 J71 J72 J73 J74 J75 J76 J77 J78 J79 J80 J81 J82 J83 J84 J85 J86 J87 J88 J89 J90 J91 J92 J93 J94 J95 J96 J97 J98 J99 J100 J101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>=Options!$J$1:$J$4</formula1>
@@ -632,13 +637,16 @@
       <formula1>=Options!$K$1:$K$5</formula1>
     </dataValidation>
     <dataValidation sqref="L2 L3 L4 L5 L6 L7 L8 L9 L10 L11 L12 L13 L14 L15 L16 L17 L18 L19 L20 L21 L22 L23 L24 L25 L26 L27 L28 L29 L30 L31 L32 L33 L34 L35 L36 L37 L38 L39 L40 L41 L42 L43 L44 L45 L46 L47 L48 L49 L50 L51 L52 L53 L54 L55 L56 L57 L58 L59 L60 L61 L62 L63 L64 L65 L66 L67 L68 L69 L70 L71 L72 L73 L74 L75 L76 L77 L78 L79 L80 L81 L82 L83 L84 L85 L86 L87 L88 L89 L90 L91 L92 L93 L94 L95 L96 L97 L98 L99 L100 L101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Options!$L$1:$L$3</formula1>
+      <formula1>=Options!$L$1:$L$4</formula1>
     </dataValidation>
     <dataValidation sqref="M2 M3 M4 M5 M6 M7 M8 M9 M10 M11 M12 M13 M14 M15 M16 M17 M18 M19 M20 M21 M22 M23 M24 M25 M26 M27 M28 M29 M30 M31 M32 M33 M34 M35 M36 M37 M38 M39 M40 M41 M42 M43 M44 M45 M46 M47 M48 M49 M50 M51 M52 M53 M54 M55 M56 M57 M58 M59 M60 M61 M62 M63 M64 M65 M66 M67 M68 M69 M70 M71 M72 M73 M74 M75 M76 M77 M78 M79 M80 M81 M82 M83 M84 M85 M86 M87 M88 M89 M90 M91 M92 M93 M94 M95 M96 M97 M98 M99 M100 M101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Options!$M$1:$M$4</formula1>
+      <formula1>=Options!$M$1:$M$5</formula1>
     </dataValidation>
     <dataValidation sqref="P2 P3 P4 P5 P6 P7 P8 P9 P10 P11 P12 P13 P14 P15 P16 P17 P18 P19 P20 P21 P22 P23 P24 P25 P26 P27 P28 P29 P30 P31 P32 P33 P34 P35 P36 P37 P38 P39 P40 P41 P42 P43 P44 P45 P46 P47 P48 P49 P50 P51 P52 P53 P54 P55 P56 P57 P58 P59 P60 P61 P62 P63 P64 P65 P66 P67 P68 P69 P70 P71 P72 P73 P74 P75 P76 P77 P78 P79 P80 P81 P82 P83 P84 P85 P86 P87 P88 P89 P90 P91 P92 P93 P94 P95 P96 P97 P98 P99 P100 P101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Options!$P$1:$P$2</formula1>
+      <formula1>=Options!$P$1:$P$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q2 Q3 Q4 Q5 Q6 Q7 Q8 Q9 Q10 Q11 Q12 Q13 Q14 Q15 Q16 Q17 Q18 Q19 Q20 Q21 Q22 Q23 Q24 Q25 Q26 Q27 Q28 Q29 Q30 Q31 Q32 Q33 Q34 Q35 Q36 Q37 Q38 Q39 Q40 Q41 Q42 Q43 Q44 Q45 Q46 Q47 Q48 Q49 Q50 Q51 Q52 Q53 Q54 Q55 Q56 Q57 Q58 Q59 Q60 Q61 Q62 Q63 Q64 Q65 Q66 Q67 Q68 Q69 Q70 Q71 Q72 Q73 Q74 Q75 Q76 Q77 Q78 Q79 Q80 Q81 Q82 Q83 Q84 Q85 Q86 Q87 Q88 Q89 Q90 Q91 Q92 Q93 Q94 Q95 Q96 Q97 Q98 Q99 Q100 Q101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=Options!$Q$1:$Q$2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -651,7 +659,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="G1:P14"/>
+  <dimension ref="G1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -697,6 +705,11 @@
       </c>
       <c r="P1" t="inlineStr">
         <is>
+          <t>soil</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
           <t>True sample</t>
         </is>
       </c>
@@ -739,6 +752,11 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
           <t>Control</t>
         </is>
       </c>
@@ -749,6 +767,11 @@
           <t>grassland</t>
         </is>
       </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>Flooded Grasslands &amp; Savannas</t>
@@ -772,6 +795,11 @@
       <c r="M3" t="inlineStr">
         <is>
           <t>Airdrying 48h+</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>marine_sediment</t>
         </is>
       </c>
     </row>
@@ -796,9 +824,19 @@
           <t>30cm-1m</t>
         </is>
       </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
       <c r="M4" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>marine_root</t>
         </is>
       </c>
     </row>
@@ -818,6 +856,11 @@
           <t>1m+</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="G6" t="inlineStr">
@@ -892,6 +935,11 @@
       </c>
     </row>
     <row r="12">
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
       <c r="I12" t="inlineStr">
         <is>
           <t>Tropical &amp; Subtropical Grasslands, Savannas &amp; Shrublands</t>
@@ -909,6 +957,13 @@
       <c r="I14" t="inlineStr">
         <is>
           <t>Tundra</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>NA</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
New template without the SequencingRun field
</commit_message>
<xml_diff>
--- a/static/xls/template_with_dropdowns_for_one_drive_and_excel.xlsx
+++ b/static/xls/template_with_dropdowns_for_one_drive_and_excel.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S101"/>
+  <dimension ref="A1:R101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,11 +509,6 @@
         </is>
       </c>
       <c r="R1" t="inlineStr">
-        <is>
-          <t>SequencingRun</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>

</xml_diff>

<commit_message>
New accepted soil depths
</commit_message>
<xml_diff>
--- a/static/xls/template_with_dropdowns_for_one_drive_and_excel.xlsx
+++ b/static/xls/template_with_dropdowns_for_one_drive_and_excel.xlsx
@@ -629,7 +629,7 @@
       <formula1>=Options!$J$1:$J$4</formula1>
     </dataValidation>
     <dataValidation sqref="K2 K3 K4 K5 K6 K7 K8 K9 K10 K11 K12 K13 K14 K15 K16 K17 K18 K19 K20 K21 K22 K23 K24 K25 K26 K27 K28 K29 K30 K31 K32 K33 K34 K35 K36 K37 K38 K39 K40 K41 K42 K43 K44 K45 K46 K47 K48 K49 K50 K51 K52 K53 K54 K55 K56 K57 K58 K59 K60 K61 K62 K63 K64 K65 K66 K67 K68 K69 K70 K71 K72 K73 K74 K75 K76 K77 K78 K79 K80 K81 K82 K83 K84 K85 K86 K87 K88 K89 K90 K91 K92 K93 K94 K95 K96 K97 K98 K99 K100 K101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Options!$K$1:$K$5</formula1>
+      <formula1>=Options!$K$1:$K$6</formula1>
     </dataValidation>
     <dataValidation sqref="L2 L3 L4 L5 L6 L7 L8 L9 L10 L11 L12 L13 L14 L15 L16 L17 L18 L19 L20 L21 L22 L23 L24 L25 L26 L27 L28 L29 L30 L31 L32 L33 L34 L35 L36 L37 L38 L39 L40 L41 L42 L43 L44 L45 L46 L47 L48 L49 L50 L51 L52 L53 L54 L55 L56 L57 L58 L59 L60 L61 L62 L63 L64 L65 L66 L67 L68 L69 L70 L71 L72 L73 L74 L75 L76 L77 L78 L79 L80 L81 L82 L83 L84 L85 L86 L87 L88 L89 L90 L91 L92 L93 L94 L95 L96 L97 L98 L99 L100 L101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>=Options!$L$1:$L$4</formula1>
@@ -685,7 +685,7 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>0-10cm</t>
+          <t>0-20cm</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
@@ -732,7 +732,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>10-20cm</t>
+          <t>20cm-40cm</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>20cm-30cm</t>
+          <t>40cm-60cm</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -816,7 +816,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>30cm-1m</t>
+          <t>60cm-80cm</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>1m+</t>
+          <t>80cm-1m</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -866,6 +866,11 @@
       <c r="I6" t="inlineStr">
         <is>
           <t>Montane Grasslands &amp; Shrublands</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>1m+</t>
         </is>
       </c>
     </row>

</xml_diff>